<commit_message>
day 2 framework code
</commit_message>
<xml_diff>
--- a/vajrang/June 2022/RoboticEnterpriseFramework_Training/Data/Config.xlsx
+++ b/vajrang/June 2022/RoboticEnterpriseFramework_Training/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uipath-my.sharepoint.com/personal/alexandra_veizu_uipath_com/Documents/Documents/Projects/FrameworkTemplates/REFramework/VB/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uipath\GitSpace\RPA-Developer-in-30-Days\vajrang\June 2022\RoboticEnterpriseFramework_Training\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F8C54E24-BA5C-4BF9-8DAB-2778512EC11B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6358CC02-1C81-48DA-99B3-7614D7B69F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10248" yWindow="17508" windowWidth="21252" windowHeight="9444" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -98,68 +98,67 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>JuneReFrameworkSampleQueue</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
   </si>
 </sst>
 </file>
@@ -537,16 +536,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -585,26 +584,26 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="28.8">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1623,12 +1622,12 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1665,7 +1664,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1673,18 +1672,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1708,7 +1707,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1730,7 +1729,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1741,7 +1740,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1752,53 +1751,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2782,16 +2781,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2802,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>